<commit_message>
reverted this to r350 since the file had somehow gotten corrupted and Excel couldn't open it (the .xls version could be opened, but the figures were broken.
git-svn-id: https://svn.mcs.anl.gov/repos/performance/orio@391 e7ad4b5f-b827-0410-872f-f7f4bc3d1efb
</commit_message>
<xml_diff>
--- a/doc/papers/cgo09/figures/experiments.xlsx
+++ b/doc/papers/cgo09/figures/experiments.xlsx
@@ -1,3 +1,253 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="-680" yWindow="-21520" windowWidth="28520" windowHeight="21000" tabRatio="500" activeTab="2"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+  </sheets>
+  <definedNames>
+    <definedName name="t" localSheetId="2">Sheet1!$A$2:$K$8</definedName>
+    <definedName name="t_1" localSheetId="2">Sheet1!$A$26:$K$98</definedName>
+    <definedName name="t_2" localSheetId="0">Sheet2!$A$1:$K$8</definedName>
+    <definedName name="t_2" localSheetId="1">Sheet3!$A$1:$K$8</definedName>
+  </definedNames>
+  <calcPr calcId="130404" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="Connection1" type="6" refreshedVersion="0">
+    <textPr fileType="mac" sourceFile="HD:Users:norris:t.csv" comma="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="Connection2" type="6" refreshedVersion="0">
+    <textPr fileType="mac" sourceFile="HD:Users:norris:t.csv" comma="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="Connection3" type="6" refreshedVersion="0">
+    <textPr fileType="mac" sourceFile="HD:Users:norris:t.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="Connection4" type="6" refreshedVersion="0">
+    <textPr fileType="mac" sourceFile="HD:Users:norris:t.csv" comma="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+  <si>
+    <t>C from Matlab</t>
+  </si>
+  <si>
+    <t>BLAS</t>
+  </si>
+  <si>
+    <t>Intel MKL</t>
+  </si>
+  <si>
+    <t>ATLAS</t>
+  </si>
+  <si>
+    <t>GEMVER Sequential</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VADD</t>
+  </si>
+  <si>
+    <t>BiCGkernel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GESUMMV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orio (Seq.)</t>
+  </si>
+  <si>
+    <t>Orio (Par.)</t>
+  </si>
+  <si>
+    <t>Orio (Par.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orio (Seq.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATLAS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orio (Par.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATAX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C from Matlab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orio (Seq.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base (Seq.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BG/P (MFLOPS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base (Par.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESSL (Seq.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESSL (Par.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goto (Seq.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goto (Par.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orio (Seq.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orio (Par.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2">
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF800080"/>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
+</styleSheet>
+</file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
@@ -11,8 +261,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.102990511721342"/>
-          <c:y val="0.185801452203708"/>
+          <c:x val="0.109824224705397"/>
+          <c:y val="0.203430674402425"/>
           <c:w val="0.865118827686403"/>
           <c:h val="0.614879507736591"/>
         </c:manualLayout>
@@ -28,7 +278,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C from MATLAB</c:v>
+                  <c:v>C from Matlab</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -596,25 +846,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="610745000"/>
-        <c:axId val="610748168"/>
+        <c:axId val="431788392"/>
+        <c:axId val="431791560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="610745000"/>
+        <c:axId val="431788392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="610748168"/>
+        <c:crossAx val="431791560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="610748168"/>
+        <c:axId val="431791560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -622,7 +872,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="610745000"/>
+        <c:crossAx val="431788392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -633,8 +883,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.150518357756533"/>
-          <c:y val="0.0139387458099364"/>
+          <c:x val="0.196076444316898"/>
+          <c:y val="0.0491971902073696"/>
           <c:w val="0.707618258244035"/>
           <c:h val="0.151329532084352"/>
         </c:manualLayout>
@@ -644,12 +894,6 @@
   </c:chart>
   <c:spPr>
     <a:ln w="9525">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
       <a:prstDash val="sysDot"/>
     </a:ln>
     <a:effectLst/>
@@ -702,7 +946,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C from MATLAB</c:v>
+                  <c:v>C from Matlab</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1270,25 +1514,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="610847160"/>
-        <c:axId val="610850328"/>
+        <c:axId val="431860792"/>
+        <c:axId val="431863960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="610847160"/>
+        <c:axId val="431860792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="610850328"/>
+        <c:crossAx val="431863960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="610850328"/>
+        <c:axId val="431863960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,7 +1540,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="610847160"/>
+        <c:crossAx val="431860792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1318,12 +1562,6 @@
   </c:chart>
   <c:spPr>
     <a:ln w="9525">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
       <a:prstDash val="sysDot"/>
     </a:ln>
     <a:effectLst/>
@@ -1376,7 +1614,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C from MATLAB</c:v>
+                  <c:v>C from Matlab</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1944,25 +2182,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="610918952"/>
-        <c:axId val="610906840"/>
+        <c:axId val="431908840"/>
+        <c:axId val="431912104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="610918952"/>
+        <c:axId val="431908840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="610906840"/>
+        <c:crossAx val="431912104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="610906840"/>
+        <c:axId val="431912104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1970,7 +2208,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="610918952"/>
+        <c:crossAx val="431908840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1992,12 +2230,6 @@
   </c:chart>
   <c:spPr>
     <a:ln w="9525">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
       <a:prstDash val="sysDot"/>
     </a:ln>
     <a:effectLst/>
@@ -2050,7 +2282,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C from MATLAB</c:v>
+                  <c:v>C from Matlab</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2618,25 +2850,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="610966600"/>
-        <c:axId val="610969944"/>
+        <c:axId val="431957032"/>
+        <c:axId val="431960232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="610966600"/>
+        <c:axId val="431957032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="610969944"/>
+        <c:crossAx val="431960232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="610969944"/>
+        <c:axId val="431960232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2644,7 +2876,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="610966600"/>
+        <c:crossAx val="431957032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2666,12 +2898,6 @@
   </c:chart>
   <c:spPr>
     <a:ln w="9525">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
       <a:prstDash val="sysDot"/>
     </a:ln>
     <a:effectLst/>
@@ -3443,25 +3669,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="611034264"/>
-        <c:axId val="611039352"/>
+        <c:axId val="451534792"/>
+        <c:axId val="451537912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="611034264"/>
+        <c:axId val="451534792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="611039352"/>
+        <c:crossAx val="451537912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="611039352"/>
+        <c:axId val="451537912"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3472,7 +3698,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="611034264"/>
+        <c:crossAx val="451534792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3503,12 +3729,6 @@
   </c:chart>
   <c:spPr>
     <a:ln w="9525">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
       <a:prstDash val="sysDot"/>
     </a:ln>
     <a:effectLst/>
@@ -3567,15 +3787,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>101599</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>98382</xdr:rowOff>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85682</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3597,15 +3817,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3627,15 +3847,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>939800</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3657,14 +3877,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4558,6 +4778,22 @@
     </cdr:sp>
   </cdr:relSizeAnchor>
 </c:userShapes>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t_2" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t_2" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="t_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4876,4 +5112,1895 @@
   </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection sqref="A1:K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C1">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="D1">
+        <v>0.17</v>
+      </c>
+      <c r="E1">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="F1">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="G1">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="H1">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="I1">
+        <v>1.2090000000000001</v>
+      </c>
+      <c r="J1">
+        <v>1.53</v>
+      </c>
+      <c r="K1">
+        <v>1.8879999999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C2">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.154</v>
+      </c>
+      <c r="E2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F2">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="G2">
+        <v>0.623</v>
+      </c>
+      <c r="H2">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="I2">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="J2">
+        <v>1.383</v>
+      </c>
+      <c r="K2">
+        <v>1.744</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D3">
+        <v>7.8E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.21</v>
+      </c>
+      <c r="G3">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="H3">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="J3">
+        <v>0.67800000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>6.3700000000000007E-2</v>
+      </c>
+      <c r="C4">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="D4">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="E4">
+        <v>1.08</v>
+      </c>
+      <c r="F4">
+        <v>1.7</v>
+      </c>
+      <c r="G4">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="H4">
+        <v>3.31</v>
+      </c>
+      <c r="I4">
+        <v>4.32</v>
+      </c>
+      <c r="J4">
+        <v>5.45</v>
+      </c>
+      <c r="K4">
+        <v>6.78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="C5">
+        <v>6.8599999999999994E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.154</v>
+      </c>
+      <c r="E5">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="F5">
+        <v>0.433</v>
+      </c>
+      <c r="G5">
+        <v>0.62</v>
+      </c>
+      <c r="H5">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="I5">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J5">
+        <v>1.39</v>
+      </c>
+      <c r="K5">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5.3499999999999999E-5</v>
+      </c>
+      <c r="C6">
+        <v>1.66E-4</v>
+      </c>
+      <c r="D6">
+        <v>3.3799999999999998E-4</v>
+      </c>
+      <c r="E6">
+        <v>5.6999999999999998E-4</v>
+      </c>
+      <c r="F6">
+        <v>8.6499999999999999E-4</v>
+      </c>
+      <c r="G6">
+        <v>1.2099999999999999E-3</v>
+      </c>
+      <c r="H6">
+        <v>1.6299999999999999E-3</v>
+      </c>
+      <c r="I6">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="J6">
+        <v>2.63E-3</v>
+      </c>
+      <c r="K6">
+        <v>2.9199999999999999E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection sqref="A1:K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C1">
+        <v>0.156</v>
+      </c>
+      <c r="D1">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="E1">
+        <v>0.625</v>
+      </c>
+      <c r="F1">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="G1">
+        <v>1.4039999999999999</v>
+      </c>
+      <c r="H1">
+        <v>1.907</v>
+      </c>
+      <c r="I1">
+        <v>2.488</v>
+      </c>
+      <c r="J1">
+        <v>3.1360000000000001</v>
+      </c>
+      <c r="K1">
+        <v>3.8690000000000002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C2">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.105</v>
+      </c>
+      <c r="E2">
+        <v>0.189</v>
+      </c>
+      <c r="F2">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="G2">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="H2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I2">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="J2">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="K2">
+        <v>1.1779999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C3">
+        <v>2.4E-2</v>
+      </c>
+      <c r="D3">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E3">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="F3">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.193</v>
+      </c>
+      <c r="H3">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="I3">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="J3">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="K3">
+        <v>0.78900000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="C4">
+        <v>8.6199999999999999E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="F4">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="G4">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="H4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I4">
+        <v>1.43</v>
+      </c>
+      <c r="J4">
+        <v>1.8</v>
+      </c>
+      <c r="K4">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="C5">
+        <v>6.8400000000000002E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.154</v>
+      </c>
+      <c r="E5">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="F5">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="I5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J5">
+        <v>1.39</v>
+      </c>
+      <c r="K5">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>9.3500000000000007E-3</v>
+      </c>
+      <c r="C6">
+        <v>4.1799999999999997E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.125</v>
+      </c>
+      <c r="E6">
+        <v>0.316</v>
+      </c>
+      <c r="F6">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="G6">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="H6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I6">
+        <v>1.51</v>
+      </c>
+      <c r="J6">
+        <v>1.9</v>
+      </c>
+      <c r="K6">
+        <v>2.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:K110"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K116" sqref="K116"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2">
+        <v>2000</v>
+      </c>
+      <c r="C2">
+        <v>4000</v>
+      </c>
+      <c r="D2">
+        <v>6000</v>
+      </c>
+      <c r="E2">
+        <v>8000</v>
+      </c>
+      <c r="F2">
+        <v>10000</v>
+      </c>
+      <c r="G2">
+        <v>12000</v>
+      </c>
+      <c r="H2">
+        <v>14000</v>
+      </c>
+      <c r="I2">
+        <v>16000</v>
+      </c>
+      <c r="J2">
+        <v>18000</v>
+      </c>
+      <c r="K2">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.157</v>
+      </c>
+      <c r="D3">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="E3">
+        <v>0.626</v>
+      </c>
+      <c r="F3">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G3">
+        <v>1.4059999999999999</v>
+      </c>
+      <c r="H3">
+        <v>1.909</v>
+      </c>
+      <c r="I3">
+        <v>2.4940000000000002</v>
+      </c>
+      <c r="J3">
+        <v>3.1429999999999998</v>
+      </c>
+      <c r="K3">
+        <v>3.8860000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C4">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="D4">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.48</v>
+      </c>
+      <c r="F4">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="G4">
+        <v>1.075</v>
+      </c>
+      <c r="H4">
+        <v>1.4470000000000001</v>
+      </c>
+      <c r="I4">
+        <v>1.899</v>
+      </c>
+      <c r="J4">
+        <v>2.3380000000000001</v>
+      </c>
+      <c r="K4">
+        <v>2.9780000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.112</v>
+      </c>
+      <c r="D5">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.42</v>
+      </c>
+      <c r="F5">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="G5">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="H5">
+        <v>1.25</v>
+      </c>
+      <c r="I5">
+        <v>1.6359999999999999</v>
+      </c>
+      <c r="J5">
+        <v>2.0630000000000002</v>
+      </c>
+      <c r="K5">
+        <v>2.5459999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="E6">
+        <v>1.091</v>
+      </c>
+      <c r="F6">
+        <v>1.7110000000000001</v>
+      </c>
+      <c r="G6">
+        <v>2.456</v>
+      </c>
+      <c r="H6">
+        <v>3.34</v>
+      </c>
+      <c r="I6">
+        <v>4.3449999999999998</v>
+      </c>
+      <c r="J6">
+        <v>5.48</v>
+      </c>
+      <c r="K6">
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C7">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="F7">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="G7">
+        <v>1.3</v>
+      </c>
+      <c r="H7">
+        <v>1.78</v>
+      </c>
+      <c r="I7">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="J7">
+        <v>2.93</v>
+      </c>
+      <c r="K7">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.159</v>
+      </c>
+      <c r="D8">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="E8">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="F8">
+        <v>1.29</v>
+      </c>
+      <c r="G8">
+        <v>1.9</v>
+      </c>
+      <c r="H8">
+        <v>2.5819999999999999</v>
+      </c>
+      <c r="I8">
+        <v>3.42</v>
+      </c>
+      <c r="J8">
+        <v>4.29</v>
+      </c>
+      <c r="K8">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="B25">
+        <v>2000</v>
+      </c>
+      <c r="C25">
+        <v>4000</v>
+      </c>
+      <c r="D25">
+        <v>6000</v>
+      </c>
+      <c r="E25">
+        <v>8000</v>
+      </c>
+      <c r="F25">
+        <v>10000</v>
+      </c>
+      <c r="G25">
+        <v>12000</v>
+      </c>
+      <c r="H25">
+        <v>14000</v>
+      </c>
+      <c r="I25">
+        <v>16000</v>
+      </c>
+      <c r="J25">
+        <v>18000</v>
+      </c>
+      <c r="K25">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0.01</v>
+      </c>
+      <c r="C26">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D26">
+        <v>0.104</v>
+      </c>
+      <c r="E26">
+        <v>0.185</v>
+      </c>
+      <c r="F26">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G26">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="H26">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="I26">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="J26">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="K26">
+        <v>1.171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C27">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="D27">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="F27">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="G27">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="H27">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="I27">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="J27">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="K27">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>9.4E-2</v>
+      </c>
+      <c r="C28">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D28">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E28">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F28">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="G28">
+        <v>0.183</v>
+      </c>
+      <c r="H28">
+        <v>0.245</v>
+      </c>
+      <c r="I28">
+        <v>0.33</v>
+      </c>
+      <c r="J28">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="K28">
+        <v>0.50900000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="C29">
+        <v>8.6300000000000002E-2</v>
+      </c>
+      <c r="D29">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="E29">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="F29">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="G29">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="H29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I29">
+        <v>1.43</v>
+      </c>
+      <c r="J29">
+        <v>1.82</v>
+      </c>
+      <c r="K29">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>2.46E-2</v>
+      </c>
+      <c r="C30">
+        <v>6.88E-2</v>
+      </c>
+      <c r="D30">
+        <v>0.154</v>
+      </c>
+      <c r="E30">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="F30">
+        <v>0.432</v>
+      </c>
+      <c r="G30">
+        <v>0.62</v>
+      </c>
+      <c r="H30">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="I30">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J30">
+        <v>1.39</v>
+      </c>
+      <c r="K30">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>9.2700000000000005E-3</v>
+      </c>
+      <c r="C31">
+        <v>4.1500000000000002E-2</v>
+      </c>
+      <c r="D31">
+        <v>0.129</v>
+      </c>
+      <c r="E31">
+        <v>0.317</v>
+      </c>
+      <c r="F31">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="G31">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="H31">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I31">
+        <v>1.53</v>
+      </c>
+      <c r="J31">
+        <v>1.65</v>
+      </c>
+      <c r="K31">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="B46">
+        <v>2000</v>
+      </c>
+      <c r="C46">
+        <v>4000</v>
+      </c>
+      <c r="D46">
+        <v>6000</v>
+      </c>
+      <c r="E46">
+        <v>8000</v>
+      </c>
+      <c r="F46">
+        <v>10000</v>
+      </c>
+      <c r="G46">
+        <v>12000</v>
+      </c>
+      <c r="H46">
+        <v>14000</v>
+      </c>
+      <c r="I46">
+        <v>16000</v>
+      </c>
+      <c r="J46">
+        <v>18000</v>
+      </c>
+      <c r="K46">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C47">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="D47">
+        <v>0.17</v>
+      </c>
+      <c r="E47">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="F47">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="G47">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="H47">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="I47">
+        <v>1.2090000000000001</v>
+      </c>
+      <c r="J47">
+        <v>1.53</v>
+      </c>
+      <c r="K47">
+        <v>1.8879999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C48">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="D48">
+        <v>0.154</v>
+      </c>
+      <c r="E48">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F48">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="G48">
+        <v>0.623</v>
+      </c>
+      <c r="H48">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="I48">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="J48">
+        <v>1.383</v>
+      </c>
+      <c r="K48">
+        <v>1.744</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C49">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D49">
+        <v>7.8E-2</v>
+      </c>
+      <c r="E49">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F49">
+        <v>0.21</v>
+      </c>
+      <c r="G49">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="H49">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="I49">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="J49">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="K49">
+        <v>0.83299999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>6.3700000000000007E-2</v>
+      </c>
+      <c r="C50">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="D50">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="E50">
+        <v>1.08</v>
+      </c>
+      <c r="F50">
+        <v>1.7</v>
+      </c>
+      <c r="G50">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="H50">
+        <v>3.31</v>
+      </c>
+      <c r="I50">
+        <v>4.32</v>
+      </c>
+      <c r="J50">
+        <v>5.45</v>
+      </c>
+      <c r="K50">
+        <v>6.78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="C51">
+        <v>6.8599999999999994E-2</v>
+      </c>
+      <c r="D51">
+        <v>0.154</v>
+      </c>
+      <c r="E51">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="F51">
+        <v>0.433</v>
+      </c>
+      <c r="G51">
+        <v>0.62</v>
+      </c>
+      <c r="H51">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="I51">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J51">
+        <v>1.39</v>
+      </c>
+      <c r="K51">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1">
+        <v>5.3600000000000002E-5</v>
+      </c>
+      <c r="C52">
+        <v>1.5200000000000001E-4</v>
+      </c>
+      <c r="D52">
+        <v>3.0800000000000001E-4</v>
+      </c>
+      <c r="E52">
+        <v>5.1900000000000004E-4</v>
+      </c>
+      <c r="F52">
+        <v>8.61E-4</v>
+      </c>
+      <c r="G52">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="H52">
+        <v>1.6299999999999999E-3</v>
+      </c>
+      <c r="I52">
+        <v>1.9E-3</v>
+      </c>
+      <c r="J52">
+        <v>2.3800000000000002E-3</v>
+      </c>
+      <c r="K52">
+        <v>3.2200000000000002E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="B68">
+        <v>2000</v>
+      </c>
+      <c r="C68">
+        <v>4000</v>
+      </c>
+      <c r="D68">
+        <v>6000</v>
+      </c>
+      <c r="E68">
+        <v>8000</v>
+      </c>
+      <c r="F68">
+        <v>10000</v>
+      </c>
+      <c r="G68">
+        <v>12000</v>
+      </c>
+      <c r="H68">
+        <v>14000</v>
+      </c>
+      <c r="I68">
+        <v>16000</v>
+      </c>
+      <c r="J68">
+        <v>18000</v>
+      </c>
+      <c r="K68">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C69">
+        <v>0.156</v>
+      </c>
+      <c r="D69">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="E69">
+        <v>0.625</v>
+      </c>
+      <c r="F69">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="G69">
+        <v>1.4039999999999999</v>
+      </c>
+      <c r="H69">
+        <v>1.907</v>
+      </c>
+      <c r="I69">
+        <v>2.488</v>
+      </c>
+      <c r="J69">
+        <v>3.1360000000000001</v>
+      </c>
+      <c r="K69">
+        <v>3.8690000000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C70">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D70">
+        <v>0.105</v>
+      </c>
+      <c r="E70">
+        <v>0.189</v>
+      </c>
+      <c r="F70">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="G70">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="H70">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I70">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="J70">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="K70">
+        <v>1.1779999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C71">
+        <v>2.4E-2</v>
+      </c>
+      <c r="D71">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E71">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="F71">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G71">
+        <v>0.193</v>
+      </c>
+      <c r="H71">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="I71">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="J71">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="K71">
+        <v>0.78900000000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="C72">
+        <v>8.6199999999999999E-2</v>
+      </c>
+      <c r="D72">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="E72">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="F72">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="G72">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="H72">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I72">
+        <v>1.43</v>
+      </c>
+      <c r="J72">
+        <v>1.8</v>
+      </c>
+      <c r="K72">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="C73">
+        <v>6.8400000000000002E-2</v>
+      </c>
+      <c r="D73">
+        <v>0.154</v>
+      </c>
+      <c r="E73">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="F73">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="G73">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="H73">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="I73">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J73">
+        <v>1.39</v>
+      </c>
+      <c r="K73">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>9.3500000000000007E-3</v>
+      </c>
+      <c r="C74">
+        <v>4.1799999999999997E-2</v>
+      </c>
+      <c r="D74">
+        <v>0.125</v>
+      </c>
+      <c r="E74">
+        <v>0.316</v>
+      </c>
+      <c r="F74">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="G74">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="H74">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I74">
+        <v>1.51</v>
+      </c>
+      <c r="J74">
+        <v>1.9</v>
+      </c>
+      <c r="K74">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="B92">
+        <v>2000</v>
+      </c>
+      <c r="C92">
+        <v>4000</v>
+      </c>
+      <c r="D92">
+        <v>6000</v>
+      </c>
+      <c r="E92">
+        <v>8000</v>
+      </c>
+      <c r="F92">
+        <v>10000</v>
+      </c>
+      <c r="G92">
+        <v>12000</v>
+      </c>
+      <c r="H92">
+        <v>14000</v>
+      </c>
+      <c r="I92">
+        <v>16000</v>
+      </c>
+      <c r="J92">
+        <v>18000</v>
+      </c>
+      <c r="K92">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" t="s">
+        <v>1</v>
+      </c>
+      <c r="B96" s="1">
+        <v>1.36E-5</v>
+      </c>
+      <c r="C96" s="1">
+        <v>2.9E-5</v>
+      </c>
+      <c r="D96" s="1">
+        <v>4.2899999999999999E-5</v>
+      </c>
+      <c r="E96" s="1">
+        <v>5.7899999999999998E-5</v>
+      </c>
+      <c r="F96" s="1">
+        <v>7.1400000000000001E-5</v>
+      </c>
+      <c r="G96" s="1">
+        <v>8.6100000000000006E-5</v>
+      </c>
+      <c r="H96">
+        <v>1E-4</v>
+      </c>
+      <c r="I96">
+        <v>1.15E-4</v>
+      </c>
+      <c r="J96">
+        <v>1.3100000000000001E-4</v>
+      </c>
+      <c r="K96">
+        <v>1.46E-4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="1">
+        <v>2.0800000000000001E-5</v>
+      </c>
+      <c r="C97" s="1">
+        <v>1.2099999999999999E-5</v>
+      </c>
+      <c r="D97" s="1">
+        <v>1.6500000000000001E-5</v>
+      </c>
+      <c r="E97" s="1">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="F97" s="1">
+        <v>2.7500000000000001E-5</v>
+      </c>
+      <c r="G97" s="1">
+        <v>3.3200000000000001E-5</v>
+      </c>
+      <c r="H97" s="1">
+        <v>3.8099999999999998E-5</v>
+      </c>
+      <c r="I97" s="1">
+        <v>4.35E-5</v>
+      </c>
+      <c r="J97" s="1">
+        <v>4.9499999999999997E-5</v>
+      </c>
+      <c r="K97" s="1">
+        <v>5.5000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" s="1">
+        <v>1.27E-5</v>
+      </c>
+      <c r="C98" s="1">
+        <v>2.7800000000000001E-5</v>
+      </c>
+      <c r="D98" s="1">
+        <v>4.1499999999999999E-5</v>
+      </c>
+      <c r="E98" s="1">
+        <v>5.5699999999999999E-5</v>
+      </c>
+      <c r="F98" s="1">
+        <v>6.8899999999999994E-5</v>
+      </c>
+      <c r="G98" s="1">
+        <v>8.2700000000000004E-5</v>
+      </c>
+      <c r="H98" s="1">
+        <v>9.6700000000000006E-5</v>
+      </c>
+      <c r="I98">
+        <v>1.11E-4</v>
+      </c>
+      <c r="J98">
+        <v>1.27E-4</v>
+      </c>
+      <c r="K98">
+        <v>1.4200000000000001E-4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="B102">
+        <v>10</v>
+      </c>
+      <c r="C102">
+        <v>100</v>
+      </c>
+      <c r="D102">
+        <v>1000</v>
+      </c>
+      <c r="E102">
+        <v>10000</v>
+      </c>
+      <c r="F102">
+        <v>50000</v>
+      </c>
+      <c r="G102">
+        <v>100000</v>
+      </c>
+      <c r="H102">
+        <v>500000</v>
+      </c>
+      <c r="I102">
+        <v>1000000</v>
+      </c>
+      <c r="J102">
+        <v>5000000</v>
+      </c>
+      <c r="K102">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103">
+        <v>69.204657999999995</v>
+      </c>
+      <c r="C103">
+        <v>221.72</v>
+      </c>
+      <c r="D103">
+        <v>364.54</v>
+      </c>
+      <c r="E103">
+        <v>247.19</v>
+      </c>
+      <c r="F103">
+        <v>254.94</v>
+      </c>
+      <c r="G103">
+        <v>255.88</v>
+      </c>
+      <c r="H103">
+        <v>289.18</v>
+      </c>
+      <c r="I103">
+        <v>289</v>
+      </c>
+      <c r="J103">
+        <v>289.2</v>
+      </c>
+      <c r="K103">
+        <v>289.18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" t="s">
+        <v>19</v>
+      </c>
+      <c r="B104">
+        <v>15.14</v>
+      </c>
+      <c r="C104">
+        <v>122.53</v>
+      </c>
+      <c r="D104">
+        <v>695.77</v>
+      </c>
+      <c r="E104">
+        <v>834.75</v>
+      </c>
+      <c r="F104">
+        <v>984.1</v>
+      </c>
+      <c r="G104">
+        <v>1003.73</v>
+      </c>
+      <c r="H104">
+        <v>1151.7</v>
+      </c>
+      <c r="I104">
+        <v>1150</v>
+      </c>
+      <c r="J104">
+        <v>1154.57</v>
+      </c>
+      <c r="K104">
+        <v>1153.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" t="s">
+        <v>20</v>
+      </c>
+      <c r="I105">
+        <v>473.21</v>
+      </c>
+      <c r="J105">
+        <v>487.49</v>
+      </c>
+      <c r="K105">
+        <v>488.23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106" t="s">
+        <v>21</v>
+      </c>
+      <c r="I106">
+        <v>831.31</v>
+      </c>
+      <c r="J106">
+        <v>856.25</v>
+      </c>
+      <c r="K106">
+        <v>858.71</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107" t="s">
+        <v>22</v>
+      </c>
+      <c r="I107">
+        <v>408.91</v>
+      </c>
+      <c r="J107">
+        <v>411.55</v>
+      </c>
+      <c r="K107">
+        <v>411.78</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="A108" t="s">
+        <v>23</v>
+      </c>
+      <c r="I108">
+        <v>408.91</v>
+      </c>
+      <c r="J108">
+        <v>411.54</v>
+      </c>
+      <c r="K108">
+        <v>411.77</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="A109" t="s">
+        <v>24</v>
+      </c>
+      <c r="B109">
+        <v>6744.61</v>
+      </c>
+      <c r="C109">
+        <v>1910.63</v>
+      </c>
+      <c r="D109">
+        <v>1902.67</v>
+      </c>
+      <c r="E109">
+        <v>781.26</v>
+      </c>
+      <c r="F109">
+        <v>781.26</v>
+      </c>
+      <c r="G109">
+        <v>781.27</v>
+      </c>
+      <c r="H109">
+        <v>544.49</v>
+      </c>
+      <c r="I109">
+        <v>534.09</v>
+      </c>
+      <c r="J109">
+        <v>537.54</v>
+      </c>
+      <c r="K109">
+        <v>533.59</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
+      <c r="A110" t="s">
+        <v>25</v>
+      </c>
+      <c r="B110">
+        <v>6739.19</v>
+      </c>
+      <c r="C110">
+        <v>1910.63</v>
+      </c>
+      <c r="D110">
+        <v>842.6</v>
+      </c>
+      <c r="E110">
+        <v>1285.72</v>
+      </c>
+      <c r="F110">
+        <v>1719.88</v>
+      </c>
+      <c r="G110">
+        <v>1739.13</v>
+      </c>
+      <c r="H110">
+        <v>1547.58</v>
+      </c>
+      <c r="I110">
+        <v>1482.57</v>
+      </c>
+      <c r="J110">
+        <v>1678.11</v>
+      </c>
+      <c r="K110">
+        <v>1511.44</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>